<commit_message>
Edited time entries in TestProcedure_detailed.xlsx Edited TestProcedure_xlsRead.m to initialize variables Removed sample time conversion in INTEGRATION_TEST_01.mdl
</commit_message>
<xml_diff>
--- a/CaseStudies/Test Procedure Scripts and Excel File/TestProcedure_detailed.xlsx
+++ b/CaseStudies/Test Procedure Scripts and Excel File/TestProcedure_detailed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="26655" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="26655" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
-        <v>3.472222222222222E-3</v>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>15</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>6.9444444444444441E-3</v>
+        <v>2.3148148148148147E-5</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>44</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
-        <v>1.0416666666666666E-2</v>
+        <v>3.4722222222222222E-5</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>18</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
-        <v>1.3888888888888888E-2</v>
+        <v>4.6296296296296294E-5</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>44</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>1.7361111111111112E-2</v>
+        <v>5.7870370370370366E-5</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>20</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
-        <v>2.0833333333333332E-2</v>
+        <v>6.9444444444444444E-5</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>22</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>2.4305555555555556E-2</v>
+        <v>8.1018518518518516E-5</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>24</v>

</xml_diff>